<commit_message>
Changed the status of IT6 in the integration plan
</commit_message>
<xml_diff>
--- a/Diagrammer/Integration plan.xlsx
+++ b/Diagrammer/Integration plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\Repos\Microwave-Oven\Diagrammer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41EE56D-2E92-4D57-A12A-4BDDD8462EE6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7B1A20-8848-49C4-A9AF-DD9F357C31AD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1EFFB5E9-297A-4BEF-91C1-B36BCFB3E832}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{1EFFB5E9-297A-4BEF-91C1-B36BCFB3E832}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -549,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D964D538-569C-477D-AB29-09EE7F562F68}">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -825,8 +825,8 @@
       <c r="L7" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="4" t="s">
-        <v>31</v>
+      <c r="M7" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Step 3 done ?
</commit_message>
<xml_diff>
--- a/Diagrammer/Integration plan.xlsx
+++ b/Diagrammer/Integration plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\Repos\Microwave-Oven\Diagrammer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruger\Desktop\Microwave-Oven\Diagrammer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5F7C52-C064-4C57-B0DB-0769B1694A2D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5904900D-BCA5-4ACD-90E9-C281609C3667}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{1EFFB5E9-297A-4BEF-91C1-B36BCFB3E832}"/>
   </bookViews>
@@ -23,7 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="33">
   <si>
     <t>Step#</t>
   </si>
@@ -127,13 +126,16 @@
   </si>
   <si>
     <t>Påbegyndt</t>
+  </si>
+  <si>
+    <t>Usikker på om der skal flere tests</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,8 +151,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,6 +178,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -179,10 +193,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -190,9 +205,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Ugyldig" xfId="1" builtinId="27"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -550,7 +567,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,8 +760,8 @@
       <c r="L5" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="4" t="s">
-        <v>31</v>
+      <c r="M5" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added IT7 Test (done)
</commit_message>
<xml_diff>
--- a/Diagrammer/Integration plan.xlsx
+++ b/Diagrammer/Integration plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\Repos\Microwave-Oven\Diagrammer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5F7C52-C064-4C57-B0DB-0769B1694A2D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90EC03B9-F221-4E1E-8D26-5F183E16A589}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{1EFFB5E9-297A-4BEF-91C1-B36BCFB3E832}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="32">
   <si>
     <t>Step#</t>
   </si>
@@ -549,7 +549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D964D538-569C-477D-AB29-09EE7F562F68}">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
@@ -866,6 +866,9 @@
       <c r="L8" t="s">
         <v>13</v>
       </c>
+      <c r="M8" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="1">

</xml_diff>

<commit_message>
Changed the integration plan
</commit_message>
<xml_diff>
--- a/Diagrammer/Integration plan.xlsx
+++ b/Diagrammer/Integration plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruger\Desktop\Microwave-Oven\Diagrammer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\Repos\Microwave-Oven\Diagrammer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5904900D-BCA5-4ACD-90E9-C281609C3667}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36026076-3C59-4924-AE9D-3554106E5ED8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{1EFFB5E9-297A-4BEF-91C1-B36BCFB3E832}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1EFFB5E9-297A-4BEF-91C1-B36BCFB3E832}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="22">
   <si>
     <t>Step#</t>
   </si>
@@ -89,40 +89,7 @@
     <t>Start-CancelButton</t>
   </si>
   <si>
-    <t>Jeg er dog i tvivl om</t>
-  </si>
-  <si>
-    <t>hvilken rækkefølge</t>
-  </si>
-  <si>
-    <t>Her skal alle buttons og door</t>
-  </si>
-  <si>
-    <t>door testes</t>
-  </si>
-  <si>
-    <t>der er bedst at gøre</t>
-  </si>
-  <si>
     <t>Done</t>
-  </si>
-  <si>
-    <t>det i - Test jer frem</t>
-  </si>
-  <si>
-    <t>Og se hvilken rækkefølge</t>
-  </si>
-  <si>
-    <t>det giver bedste</t>
-  </si>
-  <si>
-    <t>mening at teste i</t>
-  </si>
-  <si>
-    <t>skriv den rækk</t>
-  </si>
-  <si>
-    <t>efølge i tester i ind her</t>
   </si>
   <si>
     <t>Påbegyndt</t>
@@ -567,7 +534,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -647,7 +614,7 @@
         <v>13</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="N2" t="s">
         <v>10</v>
@@ -676,7 +643,7 @@
         <v>13</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="N3" t="s">
         <v>11</v>
@@ -720,7 +687,7 @@
         <v>13</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -761,7 +728,7 @@
         <v>13</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -802,7 +769,7 @@
         <v>13</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -843,7 +810,7 @@
         <v>13</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -883,27 +850,69 @@
       <c r="L8" t="s">
         <v>13</v>
       </c>
+      <c r="M8" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
       </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F10" t="s">
-        <v>22</v>
+        <v>14</v>
+      </c>
+      <c r="G10" t="s">
+        <v>14</v>
       </c>
       <c r="H10" t="s">
         <v>14</v>
@@ -926,16 +935,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
+        <v>14</v>
       </c>
       <c r="H11" t="s">
         <v>14</v>
@@ -958,16 +973,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
       </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>25</v>
+        <v>14</v>
+      </c>
+      <c r="G12" t="s">
+        <v>14</v>
       </c>
       <c r="H12" t="s">
         <v>14</v>
@@ -982,37 +1003,55 @@
         <v>14</v>
       </c>
       <c r="L12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F13" t="s">
-        <v>27</v>
+        <v>14</v>
+      </c>
+      <c r="G13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L13" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="E14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
-      </c>
-      <c r="E15" t="s">
-        <v>30</v>
       </c>
       <c r="N15">
         <v>3</v>

</xml_diff>

<commit_message>
Changed the status on the integration plan
</commit_message>
<xml_diff>
--- a/Diagrammer/Integration plan.xlsx
+++ b/Diagrammer/Integration plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\Repos\Microwave-Oven\Diagrammer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36026076-3C59-4924-AE9D-3554106E5ED8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0859A4-D2A3-4571-BAFE-319BFA8A8C98}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1EFFB5E9-297A-4BEF-91C1-B36BCFB3E832}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="22">
   <si>
     <t>Step#</t>
   </si>
@@ -534,7 +534,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -891,6 +891,9 @@
       <c r="L9" t="s">
         <v>13</v>
       </c>
+      <c r="M9" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="1">

</xml_diff>

<commit_message>
Changed the integration plan... again
</commit_message>
<xml_diff>
--- a/Diagrammer/Integration plan.xlsx
+++ b/Diagrammer/Integration plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\Repos\Microwave-Oven\Diagrammer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0859A4-D2A3-4571-BAFE-319BFA8A8C98}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADCA54B-04C4-474A-9B8D-E44FCC3DD0FC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1EFFB5E9-297A-4BEF-91C1-B36BCFB3E832}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="22">
   <si>
     <t>Step#</t>
   </si>
@@ -534,7 +534,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -932,6 +932,9 @@
       <c r="L10" t="s">
         <v>13</v>
       </c>
+      <c r="M10" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="1">

</xml_diff>

<commit_message>
Changed the IT8 test
</commit_message>
<xml_diff>
--- a/Diagrammer/Integration plan.xlsx
+++ b/Diagrammer/Integration plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\Repos\Microwave-Oven\Diagrammer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADCA54B-04C4-474A-9B8D-E44FCC3DD0FC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0B5835-0BDB-4639-8394-A27F6FDC2644}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1EFFB5E9-297A-4BEF-91C1-B36BCFB3E832}"/>
   </bookViews>
@@ -534,7 +534,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -859,22 +859,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
         <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" t="s">
-        <v>14</v>
       </c>
       <c r="H9" t="s">
         <v>14</v>
@@ -900,19 +900,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
         <v>12</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" t="s">
-        <v>14</v>
       </c>
       <c r="G10" t="s">
         <v>14</v>
@@ -941,13 +941,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
         <v>12</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" t="s">
-        <v>14</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
@@ -979,16 +979,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
         <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" t="s">
-        <v>14</v>
       </c>
       <c r="F12" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Step 10 is done
</commit_message>
<xml_diff>
--- a/Diagrammer/Integration plan.xlsx
+++ b/Diagrammer/Integration plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\Repos\Microwave-Oven\Diagrammer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruger\Desktop\Microwave-Oven\Diagrammer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC6D8C3-9F57-45DB-9C06-F7CB46265126}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2411CE1-4E0B-4F00-A16A-1BFC98D1F296}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1EFFB5E9-297A-4BEF-91C1-B36BCFB3E832}"/>
   </bookViews>
@@ -534,7 +534,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Changed the test status on the integration plan
</commit_message>
<xml_diff>
--- a/Diagrammer/Integration plan.xlsx
+++ b/Diagrammer/Integration plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruger\Desktop\Microwave-Oven\Diagrammer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\Repos\Microwave-Oven\Diagrammer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2778CBEB-83EF-44E1-91DC-4AA16B176A97}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22871440-B1CD-4B10-9465-F0064EDDEC80}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1EFFB5E9-297A-4BEF-91C1-B36BCFB3E832}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{1EFFB5E9-297A-4BEF-91C1-B36BCFB3E832}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="20">
   <si>
     <t>Step#</t>
   </si>
@@ -90,19 +90,13 @@
   </si>
   <si>
     <t>Done</t>
-  </si>
-  <si>
-    <t>Påbegyndt</t>
-  </si>
-  <si>
-    <t>Usikker på om der skal flere tests</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,15 +112,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,17 +126,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -160,23 +136,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Ugyldig" xfId="1" builtinId="27"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -533,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D964D538-569C-477D-AB29-09EE7F562F68}">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -686,8 +658,8 @@
       <c r="L4" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="4" t="s">
-        <v>20</v>
+      <c r="M4" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -727,8 +699,8 @@
       <c r="L5" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="5" t="s">
-        <v>21</v>
+      <c r="M5" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -1013,6 +985,9 @@
       </c>
       <c r="L12" t="s">
         <v>13</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Upload pictures for the journal
</commit_message>
<xml_diff>
--- a/Diagrammer/Integration plan.xlsx
+++ b/Diagrammer/Integration plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\Repos\Microwave-Oven\Diagrammer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22871440-B1CD-4B10-9465-F0064EDDEC80}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFAE96A-6DD1-4AB4-909E-5510EA807970}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{1EFFB5E9-297A-4BEF-91C1-B36BCFB3E832}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1EFFB5E9-297A-4BEF-91C1-B36BCFB3E832}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="19">
   <si>
     <t>Step#</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>Start-CancelButton</t>
-  </si>
-  <si>
-    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -122,7 +119,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -186,8 +183,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0A4827DF-BC68-4B82-A085-4D05D0970E17}" name="Tabel5" displayName="Tabel5" ref="A1:L19" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:L19" xr:uid="{1F1A0A38-A90D-4F8C-96E7-4B98CA95F6A4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0A4827DF-BC68-4B82-A085-4D05D0970E17}" name="Tabel5" displayName="Tabel5" ref="A1:L13" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:L13" xr:uid="{1F1A0A38-A90D-4F8C-96E7-4B98CA95F6A4}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{DA6F1097-9479-4310-8F46-B153BB9BFFC1}" name="Step#" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{F09D1308-1FA5-46E0-AB58-9EE0E2D125CC}" name="UserInterface"/>
@@ -505,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D964D538-569C-477D-AB29-09EE7F562F68}">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,9 +556,6 @@
       <c r="L1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="N1" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
@@ -585,12 +579,7 @@
       <c r="L2" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" t="s">
-        <v>10</v>
-      </c>
+      <c r="M2" s="3"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -614,12 +603,7 @@
       <c r="L3" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N3" t="s">
-        <v>11</v>
-      </c>
+      <c r="M3" s="3"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -658,9 +642,7 @@
       <c r="L4" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="M4" s="3"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -699,9 +681,7 @@
       <c r="L5" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -740,9 +720,7 @@
       <c r="L6" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="M6" s="3"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -781,9 +759,7 @@
       <c r="L7" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="M7" s="3"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -822,9 +798,7 @@
       <c r="L8" t="s">
         <v>13</v>
       </c>
-      <c r="M8" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="M8" s="3"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -863,9 +837,7 @@
       <c r="L9" t="s">
         <v>13</v>
       </c>
-      <c r="M9" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="M9" s="3"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -904,9 +876,7 @@
       <c r="L10" t="s">
         <v>13</v>
       </c>
-      <c r="M10" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="M10" s="3"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -945,9 +915,7 @@
       <c r="L11" t="s">
         <v>13</v>
       </c>
-      <c r="M11" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="M11" s="3"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -986,9 +954,7 @@
       <c r="L12" t="s">
         <v>13</v>
       </c>
-      <c r="M12" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="M12" s="3"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -1027,39 +993,31 @@
       <c r="L13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
+      <c r="M13" s="3"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>14</v>
+      <c r="A15" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="N15">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>15</v>
+      <c r="A16" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>16</v>
+      <c r="A17" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
+      <c r="A18" s="1"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
+      <c r="A19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>